<commit_message>
zmiana hasło,imie i nazwisko
</commit_message>
<xml_diff>
--- a/cmake-build-debug/loginy.xlsx
+++ b/cmake-build-debug/loginy.xlsx
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>admin@exemp.pl</t>
+  </si>
+  <si>
+    <t>WWA</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
getery imie nazwisko mail funkcja
</commit_message>
<xml_diff>
--- a/cmake-build-debug/loginy.xlsx
+++ b/cmake-build-debug/loginy.xlsx
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>WWA</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>123@mail</t>
+  </si>
+  <si>
+    <t>brak</t>
   </si>
 </sst>
 </file>
@@ -456,6 +468,26 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
naprawiona zmiana danych pracowników(bez funckcji bo nie mam pomysłu), dodane podstawowe funkcjie do kalendarza
</commit_message>
<xml_diff>
--- a/cmake-build-debug/loginy.xlsx
+++ b/cmake-build-debug/loginy.xlsx
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>wkow</t>
+  </si>
+  <si>
+    <t>Mati</t>
   </si>
 </sst>
 </file>
@@ -485,7 +488,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Quick fix - with sending emails and registration
</commit_message>
<xml_diff>
--- a/cmake-build-debug/loginy.xlsx
+++ b/cmake-build-debug/loginy.xlsx
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>q</t>
+  </si>
+  <si>
+    <t>XD</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>mateusz.qzera@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -534,6 +543,26 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>